<commit_message>
Trained with augmented dataset
</commit_message>
<xml_diff>
--- a/docs/train_log.xlsx
+++ b/docs/train_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Oruganti/Library/CloudStorage/GoogleDrive-finmetrics0@gmail.com/My Drive/freelance/pollen_classification/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE837F-F188-E840-A9AF-82D46628F4A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5854193-3E59-004E-8BC4-875B5CD8BA07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{2CB51A96-242E-FC4B-A802-B3240F884E1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -49,6 +49,20 @@
   </si>
   <si>
     <t>aug_0.5</t>
+  </si>
+  <si>
+    <t>aug_1.0</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>1) Added dropout in the fully connected layer
+2) Reduced learning rate from 1e-4 to 5e-5
+3) train loss and accuracy are estimated on the original train dataset, not on th augment dataset</t>
+  </si>
+  <si>
+    <t>Train loss and accuracy are estimated at the end of epoch on augumented dataset</t>
   </si>
 </sst>
 </file>
@@ -93,17 +107,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,23 +444,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC61E6E-D19D-BB4C-A997-4CCA341B8B6C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,34 +478,74 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>0.87708299999999995</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>0.5</v>
       </c>
+      <c r="D3" s="6">
+        <v>0.84679700000000002</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.85833300000000001</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rescaled the images to [-1, 1]
</commit_message>
<xml_diff>
--- a/docs/train_log.xlsx
+++ b/docs/train_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Oruganti/Library/CloudStorage/GoogleDrive-finmetrics0@gmail.com/My Drive/freelance/pollen_classification/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5854193-3E59-004E-8BC4-875B5CD8BA07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18FF2BD-4A9C-E94F-958C-8B237251D9CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{2CB51A96-242E-FC4B-A802-B3240F884E1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>aug_0.5</t>
+  </si>
+  <si>
+    <t>aug_0.5_v2</t>
   </si>
   <si>
     <t>aug_1.0</t>
@@ -59,10 +62,14 @@
   <si>
     <t>1) Added dropout in the fully connected layer
 2) Reduced learning rate from 1e-4 to 5e-5
-3) train loss and accuracy are estimated on the original train dataset, not on th augment dataset</t>
-  </si>
-  <si>
-    <t>Train loss and accuracy are estimated at the end of epoch on augumented dataset</t>
+3) train loss and accuracy are estimated on the original train dataset, not on the augment dataset</t>
+  </si>
+  <si>
+    <t>1) Max rotation increased from 30 to 135
+2) Rescaled image fro [0, 1] to [-1, 1] range</t>
+  </si>
+  <si>
+    <t>Train loss and accuracy are estimated at the end of epoch on augumented dataset. LR 1e-4</t>
   </si>
 </sst>
 </file>
@@ -87,12 +94,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -129,6 +142,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,7 +464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -458,7 +474,7 @@
     <col min="3" max="3" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="48.5" style="7" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -479,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -516,7 +532,7 @@
         <v>0.85833300000000001</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -524,20 +540,40 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="6">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.85833300000000001</v>
+      </c>
       <c r="F4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.95821699999999999</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>

</xml_diff>